<commit_message>
Additional elements added to Booking Report and Custody Query Results.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Custody_Query_Results-Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Custody_Query_Results-Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="0" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="4540" yWindow="2240" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Custody Query Results Mappin" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="142">
   <si>
     <t>Race</t>
   </si>
@@ -418,13 +418,47 @@
   </si>
   <si>
     <t>Don't Use</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>Case Court Name</t>
+  </si>
+  <si>
+    <t>Person Primary Language</t>
+  </si>
+  <si>
+    <t>Arrest Location LAT</t>
+  </si>
+  <si>
+    <t>Arrest Location Long</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Case[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:CaseAugmentation/j:CaseCourt/j:CourtName</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Person[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonPrimaryLanguage/nc:LanguageName</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Location[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Arrest/j:ArrestLocation/@structures:ref]/nc:Location2DGeospatialCoordinate/nc:GeographicCoordinateLatitude/nc:LatitudeDegreeValue</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Location[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Arrest/j:ArrestLocation/@structures:ref]/nc:Location2DGeospatialCoordinate/nc:GeographicCoordinateLongitude/nc:LongitudeDegreeValue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -515,6 +549,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF555555"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -551,663 +590,675 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="649">
+  <cellStyleXfs count="661">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1219,7 +1270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1228,25 +1279,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1255,25 +1306,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1282,17 +1333,56 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="649">
+  <cellStyles count="661">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1617,6 +1707,12 @@
     <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="652" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="654" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="656" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1941,6 +2037,12 @@
     <cellStyle name="Hyperlink" xfId="643" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="645" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="647" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="649" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="651" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="653" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="655" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="657" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="659" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2270,11 +2372,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M376"/>
+  <dimension ref="A1:M381"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2287,7 +2389,7 @@
     <col min="6" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -2304,7 +2406,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:12">
       <c r="A2" s="13" t="s">
         <v>5</v>
       </c>
@@ -2313,7 +2415,7 @@
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="1:10" ht="28">
+    <row r="3" spans="1:12" ht="28">
       <c r="A3" s="14"/>
       <c r="B3" s="14" t="s">
         <v>8</v>
@@ -2326,7 +2428,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:12">
       <c r="A4" s="14"/>
       <c r="B4" s="15" t="s">
         <v>6</v>
@@ -2339,7 +2441,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="2" customFormat="1">
+    <row r="5" spans="1:12" s="2" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -2353,7 +2455,7 @@
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1">
+    <row r="6" spans="1:12" s="2" customFormat="1">
       <c r="A6" s="16"/>
       <c r="B6" s="16" t="s">
         <v>26</v>
@@ -2366,7 +2468,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="2" customFormat="1">
+    <row r="7" spans="1:12" s="2" customFormat="1">
       <c r="A7" s="16"/>
       <c r="B7" s="16" t="s">
         <v>28</v>
@@ -2379,407 +2481,407 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:12" s="31" customFormat="1">
+      <c r="A8" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+    </row>
+    <row r="9" spans="1:12" s="31" customFormat="1" ht="56">
+      <c r="A9" s="32"/>
+      <c r="B9" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-    </row>
-    <row r="9" spans="1:10" ht="42">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:12" ht="42">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C11" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="14" t="s">
+      <c r="D11" s="18"/>
+      <c r="E11" s="14" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="42">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18" t="s">
+    <row r="12" spans="1:12" ht="42">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C12" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14" t="s">
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="42">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18" t="s">
+    <row r="13" spans="1:12" ht="42">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C13" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14" t="s">
+      <c r="D13" s="14"/>
+      <c r="E13" s="14" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="56">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14" t="s">
+    <row r="14" spans="1:12" ht="56">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C14" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="14" t="s">
+      <c r="D14" s="18"/>
+      <c r="E14" s="14" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="56">
-      <c r="A13" s="19"/>
-      <c r="B13" s="20" t="s">
+    <row r="15" spans="1:12" ht="56">
+      <c r="A15" s="19"/>
+      <c r="B15" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C15" s="15" t="s">
         <v>74</v>
-      </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="56">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="56">
-      <c r="A15" s="15"/>
-      <c r="B15" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>78</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="42">
+        <v>104</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="56">
       <c r="A16" s="15"/>
       <c r="B16" s="15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="42">
-      <c r="A17" s="20"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="56">
+      <c r="A17" s="15"/>
       <c r="B17" s="20" t="s">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="42">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="42">
+      <c r="A19" s="20"/>
+      <c r="B19" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="45">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6" t="s">
+    <row r="20" spans="1:12" ht="45">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C20" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21" t="s">
+      <c r="D20" s="21"/>
+      <c r="E20" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="13" t="s">
+    <row r="21" spans="1:12" s="31" customFormat="1" ht="60">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-    </row>
-    <row r="20" spans="1:13" ht="42">
-      <c r="A20" s="16"/>
-      <c r="B20" s="20" t="s">
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" spans="1:12" ht="42">
+      <c r="A23" s="16"/>
+      <c r="B23" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C23" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="22" t="s">
+      <c r="D23" s="16"/>
+      <c r="E23" s="22" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="42">
-      <c r="A21" s="16"/>
-      <c r="B21" s="15" t="s">
+    <row r="24" spans="1:12" ht="42">
+      <c r="A24" s="16"/>
+      <c r="B24" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C24" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="22" t="s">
+      <c r="D24" s="16"/>
+      <c r="E24" s="22" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="75">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8" t="s">
+    <row r="25" spans="1:12" ht="75">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C25" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="23" t="s">
+      <c r="D25" s="8"/>
+      <c r="E25" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F25" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="13" t="s">
+    <row r="26" spans="1:12">
+      <c r="A26" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-    </row>
-    <row r="24" spans="1:13" ht="28">
-      <c r="A24" s="24"/>
-      <c r="B24" s="18" t="s">
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+    </row>
+    <row r="27" spans="1:12" ht="28">
+      <c r="A27" s="24"/>
+      <c r="B27" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C27" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14" t="s">
+      <c r="D27" s="14"/>
+      <c r="E27" s="14" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="42">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14" t="s">
+    <row r="28" spans="1:12" ht="42">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C28" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="14" t="s">
+      <c r="D28" s="18"/>
+      <c r="E28" s="14" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="56">
-      <c r="A26" s="16"/>
-      <c r="B26" s="20" t="s">
+    <row r="29" spans="1:12" ht="56">
+      <c r="A29" s="16"/>
+      <c r="B29" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C29" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="14" t="s">
+      <c r="D29" s="16"/>
+      <c r="E29" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="13" t="s">
+    <row r="30" spans="1:12">
+      <c r="A30" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-    </row>
-    <row r="28" spans="1:13" ht="42">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21" t="s">
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+    </row>
+    <row r="31" spans="1:12" ht="42">
+      <c r="A31" s="21"/>
+      <c r="B31" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="15" t="s">
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F31" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="42">
-      <c r="A29" s="25"/>
-      <c r="B29" s="20" t="s">
+    <row r="32" spans="1:12" ht="42">
+      <c r="A32" s="25"/>
+      <c r="B32" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C32" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="15" t="s">
+      <c r="D32" s="25"/>
+      <c r="E32" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F32" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="3" t="s">
+    <row r="33" spans="1:13">
+      <c r="A33" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-    </row>
-    <row r="31" spans="1:13" ht="42">
-      <c r="A31" s="16"/>
-      <c r="B31" s="20" t="s">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+    </row>
+    <row r="34" spans="1:13" ht="42">
+      <c r="A34" s="16"/>
+      <c r="B34" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C34" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="14" t="s">
+      <c r="D34" s="16"/>
+      <c r="E34" s="14" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="42">
-      <c r="A32" s="16"/>
-      <c r="B32" s="15" t="s">
+    <row r="35" spans="1:13" ht="42">
+      <c r="A35" s="16"/>
+      <c r="B35" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C35" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="14" t="s">
+      <c r="D35" s="16"/>
+      <c r="E35" s="14" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="56">
-      <c r="A33" s="16"/>
-      <c r="B33" s="15" t="s">
+    <row r="36" spans="1:13" ht="56">
+      <c r="A36" s="16"/>
+      <c r="B36" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C36" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D33" s="16"/>
-      <c r="E33" s="14" t="s">
+      <c r="D36" s="16"/>
+      <c r="E36" s="14" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="2" customFormat="1" ht="105">
-      <c r="A34" s="7"/>
-      <c r="B34" s="8" t="s">
+    <row r="37" spans="1:13" s="2" customFormat="1" ht="105">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C37" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="9"/>
-      <c r="E34" s="8" t="s">
+      <c r="D37" s="9"/>
+      <c r="E37" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
-    </row>
-    <row r="35" spans="1:12" s="2" customFormat="1" ht="42">
-      <c r="A35" s="7"/>
-      <c r="B35" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="16"/>
-    </row>
-    <row r="36" spans="1:12">
-      <c r="A36" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:12" s="2" customFormat="1" ht="60">
-      <c r="A37" s="7"/>
-      <c r="B37" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D37" s="9"/>
-      <c r="E37" s="5" t="s">
-        <v>121</v>
       </c>
       <c r="F37" s="16" t="s">
         <v>38</v>
@@ -2791,219 +2893,271 @@
       <c r="K37" s="16"/>
       <c r="L37" s="16"/>
     </row>
-    <row r="38" spans="1:12" ht="60">
-      <c r="A38" s="10"/>
-      <c r="B38" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="F38" s="4" t="s">
+    <row r="38" spans="1:13" s="2" customFormat="1" ht="42">
+      <c r="A38" s="7"/>
+      <c r="B38" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:12" ht="56">
-      <c r="A40" s="16"/>
-      <c r="B40" s="15" t="s">
+    <row r="40" spans="1:13" s="2" customFormat="1" ht="60">
+      <c r="A40" s="7"/>
+      <c r="B40" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+    </row>
+    <row r="41" spans="1:13" s="31" customFormat="1" ht="60">
+      <c r="A41" s="7"/>
+      <c r="B41" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F41" s="40"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="40"/>
+      <c r="L41" s="40"/>
+    </row>
+    <row r="42" spans="1:13" s="31" customFormat="1" ht="60">
+      <c r="A42" s="7"/>
+      <c r="B42" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F42" s="40"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="40"/>
+      <c r="L42" s="40"/>
+    </row>
+    <row r="43" spans="1:13" ht="60">
+      <c r="A43" s="10"/>
+      <c r="B43" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:13" ht="56">
+      <c r="A45" s="16"/>
+      <c r="B45" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E40" s="22" t="s">
+      <c r="E45" s="22" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="42">
-      <c r="A41" s="16"/>
-      <c r="B41" s="20" t="s">
+    <row r="46" spans="1:13" ht="42">
+      <c r="A46" s="16"/>
+      <c r="B46" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="22" t="s">
+      <c r="D46" s="2"/>
+      <c r="E46" s="22" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="60">
-      <c r="A42" s="10" t="s">
+    <row r="47" spans="1:13" ht="60">
+      <c r="A47" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B47" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C47" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="21" t="s">
+      <c r="D47" s="8"/>
+      <c r="E47" s="21" t="s">
         <v>124</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="60">
-      <c r="A43" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D43" s="2"/>
-      <c r="E43" s="17" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12">
-      <c r="A44" s="26"/>
-      <c r="B44" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="C44" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="D44" s="28"/>
-      <c r="E44" s="29" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="56">
-      <c r="A45" s="24"/>
-      <c r="B45" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D45" s="14"/>
-      <c r="E45" s="22" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="30">
-      <c r="A46" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D46" s="8"/>
-      <c r="E46" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="30">
-      <c r="A47" s="7"/>
-      <c r="B47" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C47" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D47" s="21"/>
-      <c r="E47" s="11" t="s">
-        <v>97</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="30">
-      <c r="A48" s="7" t="s">
+    <row r="48" spans="1:13" ht="60">
+      <c r="A48" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="26"/>
+      <c r="B49" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" s="28"/>
+      <c r="E49" s="29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="56">
+      <c r="A50" s="24"/>
+      <c r="B50" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D50" s="14"/>
+      <c r="E50" s="22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="30">
+      <c r="A51" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" s="8"/>
+      <c r="E51" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="30">
+      <c r="A52" s="7"/>
+      <c r="B52" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D52" s="21"/>
+      <c r="E52" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="30">
+      <c r="A53" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="C53" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21" t="s">
+      <c r="D53" s="21"/>
+      <c r="E53" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="F53" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="30">
-      <c r="A49" s="7" t="s">
+    <row r="54" spans="1:6" ht="30">
+      <c r="A54" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="21" t="s">
+      <c r="B54" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C49" s="21" t="s">
+      <c r="C54" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21" t="s">
+      <c r="D54" s="21"/>
+      <c r="E54" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="F49" s="4" t="s">
+      <c r="F54" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="16"/>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-    </row>
-    <row r="51" spans="1:6" hidden="1">
-      <c r="A51" s="16"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="16"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="16"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="16"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="16"/>
@@ -3012,7 +3166,7 @@
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" hidden="1">
       <c r="A56" s="16"/>
       <c r="B56" s="16"/>
       <c r="C56" s="16"/>
@@ -4475,35 +4629,35 @@
       <c r="D264" s="16"/>
       <c r="E264" s="16"/>
     </row>
-    <row r="265" spans="1:5" hidden="1">
+    <row r="265" spans="1:5">
       <c r="A265" s="16"/>
       <c r="B265" s="16"/>
       <c r="C265" s="16"/>
       <c r="D265" s="16"/>
       <c r="E265" s="16"/>
     </row>
-    <row r="266" spans="1:5" hidden="1">
+    <row r="266" spans="1:5">
       <c r="A266" s="16"/>
       <c r="B266" s="16"/>
       <c r="C266" s="16"/>
       <c r="D266" s="16"/>
       <c r="E266" s="16"/>
     </row>
-    <row r="267" spans="1:5" hidden="1">
+    <row r="267" spans="1:5">
       <c r="A267" s="16"/>
       <c r="B267" s="16"/>
       <c r="C267" s="16"/>
       <c r="D267" s="16"/>
       <c r="E267" s="16"/>
     </row>
-    <row r="268" spans="1:5" hidden="1">
+    <row r="268" spans="1:5">
       <c r="A268" s="16"/>
       <c r="B268" s="16"/>
       <c r="C268" s="16"/>
       <c r="D268" s="16"/>
       <c r="E268" s="16"/>
     </row>
-    <row r="269" spans="1:5" hidden="1">
+    <row r="269" spans="1:5">
       <c r="A269" s="16"/>
       <c r="B269" s="16"/>
       <c r="C269" s="16"/>
@@ -4573,35 +4727,35 @@
       <c r="D278" s="16"/>
       <c r="E278" s="16"/>
     </row>
-    <row r="279" spans="1:5">
+    <row r="279" spans="1:5" hidden="1">
       <c r="A279" s="16"/>
       <c r="B279" s="16"/>
       <c r="C279" s="16"/>
       <c r="D279" s="16"/>
       <c r="E279" s="16"/>
     </row>
-    <row r="280" spans="1:5">
+    <row r="280" spans="1:5" hidden="1">
       <c r="A280" s="16"/>
       <c r="B280" s="16"/>
       <c r="C280" s="16"/>
       <c r="D280" s="16"/>
       <c r="E280" s="16"/>
     </row>
-    <row r="281" spans="1:5">
+    <row r="281" spans="1:5" hidden="1">
       <c r="A281" s="16"/>
       <c r="B281" s="16"/>
       <c r="C281" s="16"/>
       <c r="D281" s="16"/>
       <c r="E281" s="16"/>
     </row>
-    <row r="282" spans="1:5">
+    <row r="282" spans="1:5" hidden="1">
       <c r="A282" s="16"/>
       <c r="B282" s="16"/>
       <c r="C282" s="16"/>
       <c r="D282" s="16"/>
       <c r="E282" s="16"/>
     </row>
-    <row r="283" spans="1:5">
+    <row r="283" spans="1:5" hidden="1">
       <c r="A283" s="16"/>
       <c r="B283" s="16"/>
       <c r="C283" s="16"/>
@@ -5259,11 +5413,46 @@
       <c r="D376" s="16"/>
       <c r="E376" s="16"/>
     </row>
+    <row r="377" spans="1:5">
+      <c r="A377" s="16"/>
+      <c r="B377" s="16"/>
+      <c r="C377" s="16"/>
+      <c r="D377" s="16"/>
+      <c r="E377" s="16"/>
+    </row>
+    <row r="378" spans="1:5">
+      <c r="A378" s="16"/>
+      <c r="B378" s="16"/>
+      <c r="C378" s="16"/>
+      <c r="D378" s="16"/>
+      <c r="E378" s="16"/>
+    </row>
+    <row r="379" spans="1:5">
+      <c r="A379" s="16"/>
+      <c r="B379" s="16"/>
+      <c r="C379" s="16"/>
+      <c r="D379" s="16"/>
+      <c r="E379" s="16"/>
+    </row>
+    <row r="380" spans="1:5">
+      <c r="A380" s="16"/>
+      <c r="B380" s="16"/>
+      <c r="C380" s="16"/>
+      <c r="D380" s="16"/>
+      <c r="E380" s="16"/>
+    </row>
+    <row r="381" spans="1:5">
+      <c r="A381" s="16"/>
+      <c r="B381" s="16"/>
+      <c r="C381" s="16"/>
+      <c r="D381" s="16"/>
+      <c r="E381" s="16"/>
+    </row>
   </sheetData>
   <sortState ref="A8:J35">
     <sortCondition ref="E8:E35"/>
   </sortState>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Added Driver License and FBI ID to Custody Query Results.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Custody_Query_Results-Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Custody_Query_Results-Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4540" yWindow="2240" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="3480" yWindow="3220" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Custody Query Results Mappin" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="149">
   <si>
     <t>Race</t>
   </si>
@@ -445,6 +445,27 @@
   </si>
   <si>
     <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Location[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Arrest/j:ArrestLocation/@structures:ref]/nc:Location2DGeospatialCoordinate/nc:GeographicCoordinateLongitude/nc:LongitudeDegreeValue</t>
+  </si>
+  <si>
+    <t>Driver's License ID</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Person[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonAugmentation/j:PersonFBIIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Person[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonAugmentation/j:DriverLicense/j:DriverLicenseCardIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Driver License ID</t>
+  </si>
+  <si>
+    <t>FBI ID</t>
+  </si>
+  <si>
+    <t>Driver License Source</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Person[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonAugmentation/j:DriverLicense/j:DriverLicenseCardIdentification/nc:IdentificationSourceText</t>
   </si>
 </sst>
 </file>
@@ -590,8 +611,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="661">
+  <cellStyleXfs count="675">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1382,7 +1417,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="661">
+  <cellStyles count="675">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1713,6 +1748,13 @@
     <cellStyle name="Followed Hyperlink" xfId="656" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="664" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="666" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="668" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="670" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="672" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2043,6 +2085,13 @@
     <cellStyle name="Hyperlink" xfId="655" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="657" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="659" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="661" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="663" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="665" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="667" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="669" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="671" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="673" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2372,11 +2421,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M381"/>
+  <dimension ref="A1:M384"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2592,347 +2641,335 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="56">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15" t="s">
-        <v>75</v>
+      <c r="A16" s="19"/>
+      <c r="B16" s="20" t="s">
+        <v>142</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>76</v>
+        <v>145</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15" t="s">
-        <v>105</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="56">
-      <c r="A17" s="15"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>78</v>
+        <v>147</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>147</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="42">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15" t="s">
-        <v>79</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="56">
+      <c r="A18" s="19"/>
+      <c r="B18" s="20" t="s">
+        <v>146</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>35</v>
+        <v>146</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="42">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20" t="s">
-        <v>1</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="56">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15" t="s">
+        <v>75</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="56">
+      <c r="A20" s="15"/>
+      <c r="B20" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="42">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="42">
+      <c r="A22" s="20"/>
+      <c r="B22" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="45">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6" t="s">
+    <row r="23" spans="1:12" ht="45">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C23" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21" t="s">
+      <c r="D23" s="21"/>
+      <c r="E23" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="31" customFormat="1" ht="60">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6" t="s">
+    <row r="24" spans="1:12" s="31" customFormat="1" ht="60">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="21" t="s">
+      <c r="C24" s="6"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="40"/>
-      <c r="L21" s="40"/>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="13" t="s">
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-    </row>
-    <row r="23" spans="1:12" ht="42">
-      <c r="A23" s="16"/>
-      <c r="B23" s="20" t="s">
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+    </row>
+    <row r="26" spans="1:12" ht="42">
+      <c r="A26" s="16"/>
+      <c r="B26" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C26" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="22" t="s">
+      <c r="D26" s="16"/>
+      <c r="E26" s="22" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="42">
-      <c r="A24" s="16"/>
-      <c r="B24" s="15" t="s">
+    <row r="27" spans="1:12" ht="42">
+      <c r="A27" s="16"/>
+      <c r="B27" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C27" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="22" t="s">
+      <c r="D27" s="16"/>
+      <c r="E27" s="22" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="75">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8" t="s">
+    <row r="28" spans="1:12" ht="75">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C28" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="23" t="s">
+      <c r="D28" s="8"/>
+      <c r="E28" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="13" t="s">
+    <row r="29" spans="1:12">
+      <c r="A29" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-    </row>
-    <row r="27" spans="1:12" ht="28">
-      <c r="A27" s="24"/>
-      <c r="B27" s="18" t="s">
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+    </row>
+    <row r="30" spans="1:12" ht="28">
+      <c r="A30" s="24"/>
+      <c r="B30" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C30" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14" t="s">
+      <c r="D30" s="14"/>
+      <c r="E30" s="14" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="42">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14" t="s">
+    <row r="31" spans="1:12" ht="42">
+      <c r="A31" s="14"/>
+      <c r="B31" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C31" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="14" t="s">
+      <c r="D31" s="18"/>
+      <c r="E31" s="14" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="56">
-      <c r="A29" s="16"/>
-      <c r="B29" s="20" t="s">
+    <row r="32" spans="1:12" ht="56">
+      <c r="A32" s="16"/>
+      <c r="B32" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C32" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="14" t="s">
+      <c r="D32" s="16"/>
+      <c r="E32" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="13" t="s">
+    <row r="33" spans="1:13">
+      <c r="A33" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-    </row>
-    <row r="31" spans="1:12" ht="42">
-      <c r="A31" s="21"/>
-      <c r="B31" s="21" t="s">
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+    </row>
+    <row r="34" spans="1:13" ht="42">
+      <c r="A34" s="21"/>
+      <c r="B34" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="15" t="s">
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F34" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="42">
-      <c r="A32" s="25"/>
-      <c r="B32" s="20" t="s">
+    <row r="35" spans="1:13" ht="42">
+      <c r="A35" s="25"/>
+      <c r="B35" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C35" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="D32" s="25"/>
-      <c r="E32" s="15" t="s">
+      <c r="D35" s="25"/>
+      <c r="E35" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F35" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="3" t="s">
+    <row r="36" spans="1:13">
+      <c r="A36" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="16"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="16"/>
-    </row>
-    <row r="34" spans="1:13" ht="42">
-      <c r="A34" s="16"/>
-      <c r="B34" s="20" t="s">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+    </row>
+    <row r="37" spans="1:13" ht="42">
+      <c r="A37" s="16"/>
+      <c r="B37" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C37" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="14" t="s">
+      <c r="D37" s="16"/>
+      <c r="E37" s="14" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="42">
-      <c r="A35" s="16"/>
-      <c r="B35" s="15" t="s">
+    <row r="38" spans="1:13" ht="42">
+      <c r="A38" s="16"/>
+      <c r="B38" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C38" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D35" s="16"/>
-      <c r="E35" s="14" t="s">
+      <c r="D38" s="16"/>
+      <c r="E38" s="14" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="56">
-      <c r="A36" s="16"/>
-      <c r="B36" s="15" t="s">
+    <row r="39" spans="1:13" ht="56">
+      <c r="A39" s="16"/>
+      <c r="B39" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C39" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="14" t="s">
+      <c r="D39" s="16"/>
+      <c r="E39" s="14" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="2" customFormat="1" ht="105">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8" t="s">
+    <row r="40" spans="1:13" s="2" customFormat="1" ht="105">
+      <c r="A40" s="7"/>
+      <c r="B40" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C40" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D37" s="9"/>
-      <c r="E37" s="8" t="s">
+      <c r="D40" s="9"/>
+      <c r="E40" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16"/>
-      <c r="L37" s="16"/>
-    </row>
-    <row r="38" spans="1:13" s="2" customFormat="1" ht="42">
-      <c r="A38" s="7"/>
-      <c r="B38" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="16"/>
-      <c r="K38" s="16"/>
-      <c r="L38" s="16"/>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:13" s="2" customFormat="1" ht="60">
-      <c r="A40" s="7"/>
-      <c r="B40" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D40" s="9"/>
-      <c r="E40" s="5" t="s">
-        <v>121</v>
       </c>
       <c r="F40" s="16" t="s">
         <v>38</v>
@@ -2944,241 +2981,271 @@
       <c r="K40" s="16"/>
       <c r="L40" s="16"/>
     </row>
-    <row r="41" spans="1:13" s="31" customFormat="1" ht="60">
+    <row r="41" spans="1:13" s="2" customFormat="1" ht="42">
       <c r="A41" s="7"/>
-      <c r="B41" s="41" t="s">
+      <c r="B41" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:13" s="2" customFormat="1" ht="60">
+      <c r="A43" s="7"/>
+      <c r="B43" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="9"/>
+      <c r="E43" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+    </row>
+    <row r="44" spans="1:13" s="31" customFormat="1" ht="60">
+      <c r="A44" s="7"/>
+      <c r="B44" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="5" t="s">
+      <c r="C44" s="9"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="F41" s="40"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="39"/>
-      <c r="J41" s="39"/>
-      <c r="K41" s="40"/>
-      <c r="L41" s="40"/>
-    </row>
-    <row r="42" spans="1:13" s="31" customFormat="1" ht="60">
-      <c r="A42" s="7"/>
-      <c r="B42" s="41" t="s">
+      <c r="F44" s="40"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="39"/>
+      <c r="K44" s="40"/>
+      <c r="L44" s="40"/>
+    </row>
+    <row r="45" spans="1:13" s="31" customFormat="1" ht="60">
+      <c r="A45" s="7"/>
+      <c r="B45" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="5" t="s">
+      <c r="C45" s="9"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="F42" s="40"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
-      <c r="K42" s="40"/>
-      <c r="L42" s="40"/>
-    </row>
-    <row r="43" spans="1:13" ht="60">
-      <c r="A43" s="10"/>
-      <c r="B43" s="21" t="s">
+      <c r="F45" s="40"/>
+      <c r="G45" s="42"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
+      <c r="K45" s="40"/>
+      <c r="L45" s="40"/>
+    </row>
+    <row r="46" spans="1:13" ht="60">
+      <c r="A46" s="10"/>
+      <c r="B46" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="21" t="s">
+      <c r="C46" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21" t="s">
+      <c r="D46" s="21"/>
+      <c r="E46" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F46" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="3" t="s">
+    <row r="47" spans="1:13">
+      <c r="A47" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="1:13" ht="56">
-      <c r="A45" s="16"/>
-      <c r="B45" s="15" t="s">
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:13" ht="56">
+      <c r="A48" s="16"/>
+      <c r="B48" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E45" s="22" t="s">
+      <c r="E48" s="22" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="42">
-      <c r="A46" s="16"/>
-      <c r="B46" s="20" t="s">
+    <row r="49" spans="1:6" ht="42">
+      <c r="A49" s="16"/>
+      <c r="B49" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="22" t="s">
+      <c r="D49" s="2"/>
+      <c r="E49" s="22" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="60">
-      <c r="A47" s="10" t="s">
+    <row r="50" spans="1:6" ht="60">
+      <c r="A50" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B50" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C50" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D47" s="8"/>
-      <c r="E47" s="21" t="s">
+      <c r="D50" s="8"/>
+      <c r="E50" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="F50" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="60">
-      <c r="A48" s="16" t="s">
+    <row r="51" spans="1:6" ht="60">
+      <c r="A51" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B51" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="17" t="s">
+      <c r="D51" s="2"/>
+      <c r="E51" s="17" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="26"/>
-      <c r="B49" s="27" t="s">
+    <row r="52" spans="1:6">
+      <c r="A52" s="26"/>
+      <c r="B52" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="C49" s="28" t="s">
+      <c r="C52" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="D49" s="28"/>
-      <c r="E49" s="29" t="s">
+      <c r="D52" s="28"/>
+      <c r="E52" s="29" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="56">
-      <c r="A50" s="24"/>
-      <c r="B50" s="18" t="s">
+    <row r="53" spans="1:6" ht="56">
+      <c r="A53" s="24"/>
+      <c r="B53" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C53" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="D50" s="14"/>
-      <c r="E50" s="22" t="s">
+      <c r="D53" s="14"/>
+      <c r="E53" s="22" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="30">
-      <c r="A51" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D51" s="8"/>
-      <c r="E51" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="30">
-      <c r="A52" s="7"/>
-      <c r="B52" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C52" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D52" s="21"/>
-      <c r="E52" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="30">
-      <c r="A53" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B53" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C53" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="30">
       <c r="A54" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B54" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C54" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D54" s="21"/>
+        <v>67</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D54" s="8"/>
       <c r="E54" s="21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F54" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="16"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-    </row>
-    <row r="56" spans="1:6" hidden="1">
-      <c r="A56" s="16"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="16"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
+    <row r="55" spans="1:6" ht="30">
+      <c r="A55" s="7"/>
+      <c r="B55" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C55" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D55" s="21"/>
+      <c r="E55" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="30">
+      <c r="A56" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="30">
+      <c r="A57" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B57" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="16"/>
@@ -3187,7 +3254,7 @@
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" hidden="1">
       <c r="A59" s="16"/>
       <c r="B59" s="16"/>
       <c r="C59" s="16"/>
@@ -4664,21 +4731,21 @@
       <c r="D269" s="16"/>
       <c r="E269" s="16"/>
     </row>
-    <row r="270" spans="1:5" hidden="1">
+    <row r="270" spans="1:5">
       <c r="A270" s="16"/>
       <c r="B270" s="16"/>
       <c r="C270" s="16"/>
       <c r="D270" s="16"/>
       <c r="E270" s="16"/>
     </row>
-    <row r="271" spans="1:5" hidden="1">
+    <row r="271" spans="1:5">
       <c r="A271" s="16"/>
       <c r="B271" s="16"/>
       <c r="C271" s="16"/>
       <c r="D271" s="16"/>
       <c r="E271" s="16"/>
     </row>
-    <row r="272" spans="1:5" hidden="1">
+    <row r="272" spans="1:5">
       <c r="A272" s="16"/>
       <c r="B272" s="16"/>
       <c r="C272" s="16"/>
@@ -4762,21 +4829,21 @@
       <c r="D283" s="16"/>
       <c r="E283" s="16"/>
     </row>
-    <row r="284" spans="1:5">
+    <row r="284" spans="1:5" hidden="1">
       <c r="A284" s="16"/>
       <c r="B284" s="16"/>
       <c r="C284" s="16"/>
       <c r="D284" s="16"/>
       <c r="E284" s="16"/>
     </row>
-    <row r="285" spans="1:5">
+    <row r="285" spans="1:5" hidden="1">
       <c r="A285" s="16"/>
       <c r="B285" s="16"/>
       <c r="C285" s="16"/>
       <c r="D285" s="16"/>
       <c r="E285" s="16"/>
     </row>
-    <row r="286" spans="1:5">
+    <row r="286" spans="1:5" hidden="1">
       <c r="A286" s="16"/>
       <c r="B286" s="16"/>
       <c r="C286" s="16"/>
@@ -5447,6 +5514,27 @@
       <c r="C381" s="16"/>
       <c r="D381" s="16"/>
       <c r="E381" s="16"/>
+    </row>
+    <row r="382" spans="1:5">
+      <c r="A382" s="16"/>
+      <c r="B382" s="16"/>
+      <c r="C382" s="16"/>
+      <c r="D382" s="16"/>
+      <c r="E382" s="16"/>
+    </row>
+    <row r="383" spans="1:5">
+      <c r="A383" s="16"/>
+      <c r="B383" s="16"/>
+      <c r="C383" s="16"/>
+      <c r="D383" s="16"/>
+      <c r="E383" s="16"/>
+    </row>
+    <row r="384" spans="1:5">
+      <c r="A384" s="16"/>
+      <c r="B384" s="16"/>
+      <c r="C384" s="16"/>
+      <c r="D384" s="16"/>
+      <c r="E384" s="16"/>
     </row>
   </sheetData>
   <sortState ref="A8:J35">

</xml_diff>

<commit_message>
Updated Custody Search Results and Custody Query Results.  Added missing elements so that all "search" results appear in "query" results.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Custody_Query_Results-Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Custody_Query_Results-Mapping.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="154">
   <si>
     <t>Race</t>
   </si>
@@ -466,6 +466,21 @@
   </si>
   <si>
     <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Person[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonAugmentation/j:DriverLicense/j:DriverLicenseCardIdentification/nc:IdentificationSourceText</t>
+  </si>
+  <si>
+    <t>Charge Count Quantity</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Charge[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:ActivityChargeAssociation/j:Charge/@structures:ref]/j:ChargeCountQuantity</t>
+  </si>
+  <si>
+    <t>Statute Section ID</t>
+  </si>
+  <si>
+    <t>Statute or Ordinance Section Number</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Charge[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:ActivityChargeAssociation/j:Charge/@structures:ref]/j:ChargeStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -611,8 +626,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="675">
+  <cellStyleXfs count="679">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1417,7 +1436,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="675">
+  <cellStyles count="679">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1755,6 +1774,8 @@
     <cellStyle name="Followed Hyperlink" xfId="670" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="672" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="676" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="678" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2092,6 +2113,8 @@
     <cellStyle name="Hyperlink" xfId="669" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="671" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="673" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="675" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="677" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2421,11 +2444,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M384"/>
+  <dimension ref="A1:M386"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2935,94 +2958,87 @@
     </row>
     <row r="38" spans="1:13" ht="42">
       <c r="A38" s="16"/>
-      <c r="B38" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>89</v>
-      </c>
+      <c r="B38" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C38" s="16"/>
       <c r="D38" s="16"/>
       <c r="E38" s="14" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="56">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="42">
       <c r="A39" s="16"/>
       <c r="B39" s="15" t="s">
-        <v>90</v>
+        <v>11</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="56">
+      <c r="A40" s="16"/>
+      <c r="B40" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="16"/>
+      <c r="E40" s="14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="56">
+      <c r="A41" s="16"/>
+      <c r="B41" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D41" s="16"/>
+      <c r="E41" s="14" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="2" customFormat="1" ht="105">
-      <c r="A40" s="7"/>
-      <c r="B40" s="8" t="s">
+    <row r="42" spans="1:13" s="2" customFormat="1" ht="105">
+      <c r="A42" s="7"/>
+      <c r="B42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C42" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D40" s="9"/>
-      <c r="E40" s="8" t="s">
+      <c r="D42" s="9"/>
+      <c r="E42" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="F40" s="16" t="s">
+      <c r="F42" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
-      <c r="I40" s="16"/>
-      <c r="J40" s="16"/>
-      <c r="K40" s="16"/>
-      <c r="L40" s="16"/>
-    </row>
-    <row r="41" spans="1:13" s="2" customFormat="1" ht="42">
-      <c r="A41" s="7"/>
-      <c r="B41" s="8" t="s">
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
+    </row>
+    <row r="43" spans="1:13" s="2" customFormat="1" ht="42">
+      <c r="A43" s="7"/>
+      <c r="B43" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="14" t="s">
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="F41" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="16"/>
-      <c r="J41" s="16"/>
-      <c r="K41" s="16"/>
-      <c r="L41" s="16"/>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:13" s="2" customFormat="1" ht="60">
-      <c r="A43" s="7"/>
-      <c r="B43" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D43" s="9"/>
-      <c r="E43" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F43" s="16" t="s">
+      <c r="F43" s="5" t="s">
         <v>38</v>
       </c>
       <c r="G43" s="16"/>
@@ -3032,234 +3048,251 @@
       <c r="K43" s="16"/>
       <c r="L43" s="16"/>
     </row>
-    <row r="44" spans="1:13" s="31" customFormat="1" ht="60">
-      <c r="A44" s="7"/>
-      <c r="B44" s="41" t="s">
+    <row r="44" spans="1:13">
+      <c r="A44" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:13" s="2" customFormat="1" ht="60">
+      <c r="A45" s="7"/>
+      <c r="B45" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45" s="9"/>
+      <c r="E45" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F45" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
+    </row>
+    <row r="46" spans="1:13" s="31" customFormat="1" ht="60">
+      <c r="A46" s="7"/>
+      <c r="B46" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="5" t="s">
+      <c r="C46" s="9"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="F44" s="40"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="39"/>
-      <c r="K44" s="40"/>
-      <c r="L44" s="40"/>
-    </row>
-    <row r="45" spans="1:13" s="31" customFormat="1" ht="60">
-      <c r="A45" s="7"/>
-      <c r="B45" s="41" t="s">
+      <c r="F46" s="40"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
+      <c r="K46" s="40"/>
+      <c r="L46" s="40"/>
+    </row>
+    <row r="47" spans="1:13" s="31" customFormat="1" ht="60">
+      <c r="A47" s="7"/>
+      <c r="B47" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="5" t="s">
+      <c r="C47" s="9"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="F45" s="40"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
-      <c r="K45" s="40"/>
-      <c r="L45" s="40"/>
-    </row>
-    <row r="46" spans="1:13" ht="60">
-      <c r="A46" s="10"/>
-      <c r="B46" s="21" t="s">
+      <c r="F47" s="40"/>
+      <c r="G47" s="42"/>
+      <c r="H47" s="42"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
+      <c r="K47" s="40"/>
+      <c r="L47" s="40"/>
+    </row>
+    <row r="48" spans="1:13" ht="60">
+      <c r="A48" s="10"/>
+      <c r="B48" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="21" t="s">
+      <c r="C48" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21" t="s">
+      <c r="D48" s="21"/>
+      <c r="E48" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="F48" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
-      <c r="A47" s="3" t="s">
+    <row r="49" spans="1:6">
+      <c r="A49" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="1:13" ht="56">
-      <c r="A48" s="16"/>
-      <c r="B48" s="15" t="s">
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" ht="56">
+      <c r="A50" s="16"/>
+      <c r="B50" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C50" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E48" s="22" t="s">
+      <c r="E50" s="22" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="42">
-      <c r="A49" s="16"/>
-      <c r="B49" s="20" t="s">
+    <row r="51" spans="1:6" ht="42">
+      <c r="A51" s="16"/>
+      <c r="B51" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D49" s="2"/>
-      <c r="E49" s="22" t="s">
+      <c r="D51" s="2"/>
+      <c r="E51" s="22" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="60">
-      <c r="A50" s="10" t="s">
+    <row r="52" spans="1:6" ht="60">
+      <c r="A52" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B52" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C52" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D50" s="8"/>
-      <c r="E50" s="21" t="s">
+      <c r="D52" s="8"/>
+      <c r="E52" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="F52" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="60">
-      <c r="A51" s="16" t="s">
+    <row r="53" spans="1:6" ht="60">
+      <c r="A53" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B53" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D51" s="2"/>
-      <c r="E51" s="17" t="s">
+      <c r="D53" s="2"/>
+      <c r="E53" s="17" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="26"/>
-      <c r="B52" s="27" t="s">
+    <row r="54" spans="1:6">
+      <c r="A54" s="26"/>
+      <c r="B54" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="C52" s="28" t="s">
+      <c r="C54" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="D52" s="28"/>
-      <c r="E52" s="29" t="s">
+      <c r="D54" s="28"/>
+      <c r="E54" s="29" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="56">
-      <c r="A53" s="24"/>
-      <c r="B53" s="18" t="s">
+    <row r="55" spans="1:6" ht="56">
+      <c r="A55" s="24"/>
+      <c r="B55" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C55" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="D53" s="14"/>
-      <c r="E53" s="22" t="s">
+      <c r="D55" s="14"/>
+      <c r="E55" s="22" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="30">
-      <c r="A54" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D54" s="8"/>
-      <c r="E54" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="30">
-      <c r="A55" s="7"/>
-      <c r="B55" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C55" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D55" s="21"/>
-      <c r="E55" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="30">
       <c r="A56" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B56" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C56" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D56" s="21"/>
+        <v>67</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D56" s="8"/>
       <c r="E56" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F56" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="30">
-      <c r="A57" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="A57" s="7"/>
       <c r="B57" s="21" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C57" s="21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D57" s="21"/>
-      <c r="E57" s="21" t="s">
-        <v>99</v>
+      <c r="E57" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="F57" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="16"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="16"/>
-    </row>
-    <row r="59" spans="1:6" hidden="1">
-      <c r="A59" s="16"/>
-      <c r="B59" s="16"/>
-      <c r="C59" s="16"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="16"/>
+    <row r="58" spans="1:6" ht="30">
+      <c r="A58" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B58" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C58" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="30">
+      <c r="A59" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B59" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="16"/>
@@ -3268,7 +3301,7 @@
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" hidden="1">
       <c r="A61" s="16"/>
       <c r="B61" s="16"/>
       <c r="C61" s="16"/>
@@ -4752,14 +4785,14 @@
       <c r="D272" s="16"/>
       <c r="E272" s="16"/>
     </row>
-    <row r="273" spans="1:5" hidden="1">
+    <row r="273" spans="1:5">
       <c r="A273" s="16"/>
       <c r="B273" s="16"/>
       <c r="C273" s="16"/>
       <c r="D273" s="16"/>
       <c r="E273" s="16"/>
     </row>
-    <row r="274" spans="1:5" hidden="1">
+    <row r="274" spans="1:5">
       <c r="A274" s="16"/>
       <c r="B274" s="16"/>
       <c r="C274" s="16"/>
@@ -4850,14 +4883,14 @@
       <c r="D286" s="16"/>
       <c r="E286" s="16"/>
     </row>
-    <row r="287" spans="1:5">
+    <row r="287" spans="1:5" hidden="1">
       <c r="A287" s="16"/>
       <c r="B287" s="16"/>
       <c r="C287" s="16"/>
       <c r="D287" s="16"/>
       <c r="E287" s="16"/>
     </row>
-    <row r="288" spans="1:5">
+    <row r="288" spans="1:5" hidden="1">
       <c r="A288" s="16"/>
       <c r="B288" s="16"/>
       <c r="C288" s="16"/>
@@ -5535,6 +5568,20 @@
       <c r="C384" s="16"/>
       <c r="D384" s="16"/>
       <c r="E384" s="16"/>
+    </row>
+    <row r="385" spans="1:5">
+      <c r="A385" s="16"/>
+      <c r="B385" s="16"/>
+      <c r="C385" s="16"/>
+      <c r="D385" s="16"/>
+      <c r="E385" s="16"/>
+    </row>
+    <row r="386" spans="1:5">
+      <c r="A386" s="16"/>
+      <c r="B386" s="16"/>
+      <c r="C386" s="16"/>
+      <c r="D386" s="16"/>
+      <c r="E386" s="16"/>
     </row>
   </sheetData>
   <sortState ref="A8:J35">

</xml_diff>

<commit_message>
Now using SupervisionReleaseElgibilityDate (Scheduled) and ReleaseDate (Actual).
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Custody_Query_Results-Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Custody_Query_Results-Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="3220" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="10780" yWindow="2660" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Custody Query Results Mappin" sheetId="1" r:id="rId1"/>
@@ -216,12 +216,6 @@
     <t>Arrest</t>
   </si>
   <si>
-    <t>Release Date/Time</t>
-  </si>
-  <si>
-    <t>Supervision Release Date</t>
-  </si>
-  <si>
     <t>x-ext-code</t>
   </si>
   <si>
@@ -300,9 +294,6 @@
     <t>br-doc:BookingReports/br-ext:BookingReport/j:Arrest/j:ArrestAgency/nc:OrganizationName</t>
   </si>
   <si>
-    <t>The date a subject is released from detention.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> The agency for whom a subject is being held. (sending agency)</t>
   </si>
   <si>
@@ -387,9 +378,6 @@
     <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Location[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Arrest/j:ArrestLocation/@structures:ref]/nc:Address/nc:AddressFullText</t>
   </si>
   <si>
-    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Detention[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionReleaseDate/nc:DateTime</t>
-  </si>
-  <si>
     <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Detention[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/nc:ActivityDate/nc:Date</t>
   </si>
   <si>
@@ -417,9 +405,6 @@
     <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Person[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonDigitalImage/nc:Base64BinaryObject</t>
   </si>
   <si>
-    <t>Don't Use</t>
-  </si>
-  <si>
     <t>Case</t>
   </si>
   <si>
@@ -481,13 +466,35 @@
   </si>
   <si>
     <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Charge[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:ActivityChargeAssociation/j:Charge/@structures:ref]/j:ChargeStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>Actual Release Date/Time</t>
+  </si>
+  <si>
+    <t>Scheduled Release Date</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Detention[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionReleaseEligibilityDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Release[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/nc:ActivityDate/nc:DateTime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -590,8 +597,16 @@
       <color rgb="FF555555"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -610,12 +625,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -626,693 +635,699 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="679">
+  <cellStyleXfs count="685">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1324,7 +1339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1333,25 +1348,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1360,40 +1375,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1402,41 +1447,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="679">
+  <cellStyles count="685">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1776,6 +1794,9 @@
     <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="676" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="678" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="682" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2115,6 +2136,9 @@
     <cellStyle name="Hyperlink" xfId="673" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="675" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="677" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="681" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2444,11 +2468,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M386"/>
+  <dimension ref="A1:M385"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2472,7 +2496,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>12</v>
@@ -2497,7 +2521,7 @@
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2510,7 +2534,7 @@
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1">
@@ -2553,38 +2577,38 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="31" customFormat="1">
+    <row r="8" spans="1:12" s="27" customFormat="1">
       <c r="A8" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+    </row>
+    <row r="9" spans="1:12" s="27" customFormat="1" ht="56">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-    </row>
-    <row r="9" spans="1:12" s="31" customFormat="1" ht="56">
-      <c r="A9" s="32"/>
-      <c r="B9" s="33" t="s">
-        <v>134</v>
-      </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="13" t="s">
@@ -2601,11 +2625,11 @@
         <v>13</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="42">
@@ -2614,11 +2638,11 @@
         <v>2</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="42">
@@ -2627,11 +2651,11 @@
         <v>0</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="56">
@@ -2640,24 +2664,24 @@
         <v>23</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="56">
       <c r="A15" s="19"/>
       <c r="B15" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>37</v>
@@ -2666,79 +2690,79 @@
     <row r="16" spans="1:12" ht="56">
       <c r="A16" s="19"/>
       <c r="B16" s="20" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="56">
       <c r="A17" s="19"/>
       <c r="B17" s="20" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="56">
       <c r="A18" s="19"/>
       <c r="B18" s="20" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="56">
       <c r="A19" s="15"/>
       <c r="B19" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="56">
       <c r="A20" s="15"/>
       <c r="B20" s="20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="42">
       <c r="A21" s="15"/>
       <c r="B21" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="42">
@@ -2747,46 +2771,46 @@
         <v>1</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="45">
       <c r="A23" s="6"/>
       <c r="B23" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="21" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="31" customFormat="1" ht="60">
+    <row r="24" spans="1:12" s="27" customFormat="1" ht="60">
       <c r="A24" s="6"/>
       <c r="B24" s="6" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C24" s="6"/>
-      <c r="D24" s="36"/>
+      <c r="D24" s="32"/>
       <c r="E24" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+        <v>134</v>
+      </c>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="13" t="s">
@@ -2803,11 +2827,11 @@
         <v>18</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="22" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="42">
@@ -2816,11 +2840,11 @@
         <v>19</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="22" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="75">
@@ -2833,7 +2857,7 @@
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>38</v>
@@ -2854,24 +2878,24 @@
         <v>14</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D30" s="14"/>
       <c r="E30" s="14" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="42">
       <c r="A31" s="14"/>
       <c r="B31" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="14" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="56">
@@ -2884,7 +2908,7 @@
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="14" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -2904,7 +2928,7 @@
       <c r="C34" s="21"/>
       <c r="D34" s="21"/>
       <c r="E34" s="15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>38</v>
@@ -2916,11 +2940,11 @@
         <v>20</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>60</v>
@@ -2949,22 +2973,22 @@
         <v>17</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="42">
       <c r="A38" s="16"/>
       <c r="B38" s="20" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
       <c r="E38" s="14" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="42">
@@ -2973,37 +2997,37 @@
         <v>11</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="56">
       <c r="A40" s="16"/>
       <c r="B40" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C40" s="16" t="s">
         <v>42</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="14" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="56">
       <c r="A41" s="16"/>
       <c r="B41" s="15" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="14" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:13" s="2" customFormat="1" ht="105">
@@ -3016,7 +3040,7 @@
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F42" s="16" t="s">
         <v>38</v>
@@ -3031,12 +3055,12 @@
     <row r="43" spans="1:13" s="2" customFormat="1" ht="42">
       <c r="A43" s="7"/>
       <c r="B43" s="8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="14" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>38</v>
@@ -3063,11 +3087,11 @@
         <v>61</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F45" s="16" t="s">
         <v>38</v>
@@ -3079,41 +3103,41 @@
       <c r="K45" s="16"/>
       <c r="L45" s="16"/>
     </row>
-    <row r="46" spans="1:13" s="31" customFormat="1" ht="60">
+    <row r="46" spans="1:13" s="27" customFormat="1" ht="60">
       <c r="A46" s="7"/>
-      <c r="B46" s="41" t="s">
+      <c r="B46" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F46" s="36"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="36"/>
+      <c r="L46" s="36"/>
+    </row>
+    <row r="47" spans="1:13" s="27" customFormat="1" ht="60">
+      <c r="A47" s="7"/>
+      <c r="B47" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" s="9"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F46" s="40"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
-      <c r="K46" s="40"/>
-      <c r="L46" s="40"/>
-    </row>
-    <row r="47" spans="1:13" s="31" customFormat="1" ht="60">
-      <c r="A47" s="7"/>
-      <c r="B47" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="F47" s="40"/>
-      <c r="G47" s="42"/>
-      <c r="H47" s="42"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
-      <c r="K47" s="40"/>
-      <c r="L47" s="40"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="35"/>
+      <c r="J47" s="35"/>
+      <c r="K47" s="36"/>
+      <c r="L47" s="36"/>
     </row>
     <row r="48" spans="1:13" ht="60">
       <c r="A48" s="10"/>
@@ -3125,152 +3149,140 @@
       </c>
       <c r="D48" s="21"/>
       <c r="E48" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:6" s="41" customFormat="1">
+      <c r="A49" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
+    </row>
+    <row r="50" spans="1:6" s="43" customFormat="1" ht="42">
+      <c r="A50" s="42"/>
+      <c r="B50" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E50" s="43" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="1:6" ht="56">
-      <c r="A50" s="16"/>
-      <c r="B50" s="15" t="s">
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="1:6" ht="42">
+      <c r="A52" s="16"/>
+      <c r="B52" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="60">
+      <c r="A53" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" s="8"/>
+      <c r="E53" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="60">
+      <c r="A54" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" s="17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="60">
+      <c r="A55" s="16"/>
+      <c r="B55" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="60">
+      <c r="A56" s="16"/>
+      <c r="B56" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="30">
+      <c r="A57" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="B57" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="8"/>
+      <c r="E57" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="E50" s="22" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="42">
-      <c r="A51" s="16"/>
-      <c r="B51" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D51" s="2"/>
-      <c r="E51" s="22" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="60">
-      <c r="A52" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D52" s="8"/>
-      <c r="E52" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="60">
-      <c r="A53" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B53" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D53" s="2"/>
-      <c r="E53" s="17" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="26"/>
-      <c r="B54" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="C54" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="D54" s="28"/>
-      <c r="E54" s="29" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="56">
-      <c r="A55" s="24"/>
-      <c r="B55" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D55" s="14"/>
-      <c r="E55" s="22" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="30">
-      <c r="A56" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D56" s="8"/>
-      <c r="E56" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="30">
-      <c r="A57" s="7"/>
-      <c r="B57" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C57" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D57" s="21"/>
-      <c r="E57" s="11" t="s">
-        <v>97</v>
       </c>
       <c r="F57" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="30">
-      <c r="A58" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="A58" s="7"/>
       <c r="B58" s="21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D58" s="21"/>
-      <c r="E58" s="21" t="s">
-        <v>98</v>
+      <c r="E58" s="11" t="s">
+        <v>94</v>
       </c>
       <c r="F58" s="4" t="s">
         <v>38</v>
@@ -3281,27 +3293,38 @@
         <v>41</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D59" s="21"/>
       <c r="E59" s="21" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F59" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="16"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="16"/>
-    </row>
-    <row r="61" spans="1:6" hidden="1">
+    <row r="60" spans="1:6" ht="30">
+      <c r="A60" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C60" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" s="16"/>
       <c r="B61" s="16"/>
       <c r="C61" s="16"/>
@@ -4792,7 +4815,7 @@
       <c r="D273" s="16"/>
       <c r="E273" s="16"/>
     </row>
-    <row r="274" spans="1:5">
+    <row r="274" spans="1:5" hidden="1">
       <c r="A274" s="16"/>
       <c r="B274" s="16"/>
       <c r="C274" s="16"/>
@@ -4890,7 +4913,7 @@
       <c r="D287" s="16"/>
       <c r="E287" s="16"/>
     </row>
-    <row r="288" spans="1:5" hidden="1">
+    <row r="288" spans="1:5">
       <c r="A288" s="16"/>
       <c r="B288" s="16"/>
       <c r="C288" s="16"/>
@@ -5576,18 +5599,11 @@
       <c r="D385" s="16"/>
       <c r="E385" s="16"/>
     </row>
-    <row r="386" spans="1:5">
-      <c r="A386" s="16"/>
-      <c r="B386" s="16"/>
-      <c r="C386" s="16"/>
-      <c r="D386" s="16"/>
-      <c r="E386" s="16"/>
-    </row>
   </sheetData>
   <sortState ref="A8:J35">
     <sortCondition ref="E8:E35"/>
   </sortState>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Added "Cell" and "Bed" to IEPD.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Custody_Query_Results-Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Custody_Query_Results-Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4840" yWindow="3980" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="3680" yWindow="420" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Custody Query Results Mappin" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="160">
   <si>
     <t>Race</t>
   </si>
@@ -481,6 +481,24 @@
   </si>
   <si>
     <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Release[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/nc:ActivityDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>Bed</t>
+  </si>
+  <si>
+    <t>An identification of a bed within a supervision facility cell a subject is assigned.</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>An identification of a cell housing within a supervision facility a subject is assigned.</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Detention[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionBedIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Detention[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionCellIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -635,7 +653,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="685">
+  <cellStyleXfs count="689">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1321,8 +1339,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1456,8 +1478,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="685">
+  <cellStyles count="689">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1800,6 +1825,8 @@
     <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="682" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="686" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="688" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2142,6 +2169,8 @@
     <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="681" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="685" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="687" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2471,11 +2500,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M385"/>
+  <dimension ref="A1:M387"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3257,89 +3286,99 @@
         <v>122</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="30">
-      <c r="A57" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D57" s="8"/>
-      <c r="E57" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="30">
-      <c r="A58" s="7"/>
-      <c r="B58" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C58" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D58" s="21"/>
-      <c r="E58" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>38</v>
+    <row r="57" spans="1:6" s="45" customFormat="1" ht="60">
+      <c r="A57" s="18"/>
+      <c r="B57" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="C57" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="E57" s="17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="45" customFormat="1" ht="60">
+      <c r="A58" s="18"/>
+      <c r="B58" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="C58" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="E58" s="17" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="30">
       <c r="A59" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B59" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C59" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D59" s="21"/>
+        <v>65</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D59" s="8"/>
       <c r="E59" s="21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F59" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="30">
-      <c r="A60" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="A60" s="7"/>
       <c r="B60" s="21" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D60" s="21"/>
-      <c r="E60" s="21" t="s">
-        <v>96</v>
+      <c r="E60" s="11" t="s">
+        <v>94</v>
       </c>
       <c r="F60" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="16"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" s="16"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
+    <row r="61" spans="1:6" ht="30">
+      <c r="A61" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B61" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="30">
+      <c r="A62" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B62" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C62" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="16"/>
@@ -4818,14 +4857,14 @@
       <c r="D273" s="16"/>
       <c r="E273" s="16"/>
     </row>
-    <row r="274" spans="1:5" hidden="1">
+    <row r="274" spans="1:5">
       <c r="A274" s="16"/>
       <c r="B274" s="16"/>
       <c r="C274" s="16"/>
       <c r="D274" s="16"/>
       <c r="E274" s="16"/>
     </row>
-    <row r="275" spans="1:5" hidden="1">
+    <row r="275" spans="1:5">
       <c r="A275" s="16"/>
       <c r="B275" s="16"/>
       <c r="C275" s="16"/>
@@ -4916,14 +4955,14 @@
       <c r="D287" s="16"/>
       <c r="E287" s="16"/>
     </row>
-    <row r="288" spans="1:5">
+    <row r="288" spans="1:5" hidden="1">
       <c r="A288" s="16"/>
       <c r="B288" s="16"/>
       <c r="C288" s="16"/>
       <c r="D288" s="16"/>
       <c r="E288" s="16"/>
     </row>
-    <row r="289" spans="1:5">
+    <row r="289" spans="1:5" hidden="1">
       <c r="A289" s="16"/>
       <c r="B289" s="16"/>
       <c r="C289" s="16"/>
@@ -5601,6 +5640,20 @@
       <c r="C385" s="16"/>
       <c r="D385" s="16"/>
       <c r="E385" s="16"/>
+    </row>
+    <row r="386" spans="1:5">
+      <c r="A386" s="16"/>
+      <c r="B386" s="16"/>
+      <c r="C386" s="16"/>
+      <c r="D386" s="16"/>
+      <c r="E386" s="16"/>
+    </row>
+    <row r="387" spans="1:5">
+      <c r="A387" s="16"/>
+      <c r="B387" s="16"/>
+      <c r="C387" s="16"/>
+      <c r="D387" s="16"/>
+      <c r="E387" s="16"/>
     </row>
   </sheetData>
   <sortState ref="A8:J35">

</xml_diff>